<commit_message>
update code for new predicitons
</commit_message>
<xml_diff>
--- a/d_1.xlsx
+++ b/d_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eng\Desktop\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB53F5BB-A2CB-4EEF-8CAA-DB449D520FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813E64B5-37B8-4208-8C5D-342AE0874495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,10 +372,21 @@
   <dimension ref="A1:I769"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I769"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
update new data from the origin, add excel files to include new bundle updates that fix issues and performance evalutaion
</commit_message>
<xml_diff>
--- a/d_1.xlsx
+++ b/d_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eng\Desktop\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813E64B5-37B8-4208-8C5D-342AE0874495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3DCDB3-02D3-4C5D-868A-6652EFC569BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -371,8 +371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I769"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A757" workbookViewId="0">
+      <selection activeCell="I772" sqref="I772"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>